<commit_message>
created Seperate TestReports tester class for executing Report functionality and also derived TestResult file from Project to make test result as generic
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite CourtOrder AEO1971civildebt201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite CourtOrder AEO1971civildebt201819.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6F820C27-6D99-4C3D-97FE-E6A8FE5CA7D5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="10_ncr:8100000_{BA5C2FF3-A9CF-4CD1-9233-254A3A3F77D3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="210" windowWidth="14340" windowHeight="4335" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3" windowHeight="4335" windowWidth="14340" xWindow="390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="210"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="TCOAEO1971civildebtSepPayroll" sheetId="2" r:id="rId2"/>
-    <sheet name="TCOAEO1971civildebtOctPayroll" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="TCOAEO1971civildebtSepPayroll" r:id="rId2" sheetId="2"/>
+    <sheet name="TCOAEO1971civildebtOctPayroll" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="53">
   <si>
     <t>TC</t>
   </si>
@@ -160,9 +160,6 @@
     <t>October-2018</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>DO NOT TOUCH AUTMN COURT ORDER REPORTS</t>
   </si>
   <si>
@@ -179,12 +176,19 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>F:\\Automation_TestResults\\Payroll_CourtOrderScenarios 201819\\201819 Payroll Court order and Student Loan Test result.xlsx</t>
+  </si>
+  <si>
+    <t>PayFrequency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,54 +241,57 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="14">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -301,10 +308,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -339,7 +346,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,7 +398,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,7 +503,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -505,13 +512,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -521,7 +528,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -530,7 +537,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -539,7 +546,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -549,12 +556,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -585,7 +592,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -604,7 +611,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -616,19 +623,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -645,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -659,7 +666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -702,88 +709,88 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="29" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row customFormat="1" r="1" s="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="8" t="s">
         <v>23</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="45" r="2" s="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -799,7 +806,7 @@
       <c r="E2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G2" s="7" t="s">
@@ -809,50 +816,56 @@
         <v>39</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="M2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="13" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -892,17 +905,26 @@
       <c r="M1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="45" r="2" s="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -918,7 +940,7 @@
       <c r="E2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G2" s="7" t="s">
@@ -928,10 +950,10 @@
         <v>39</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>25</v>
@@ -939,41 +961,52 @@
       <c r="L2" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="M2" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="N2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="39.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="14" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1008,13 +1041,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -1026,7 +1059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="48.75" r="2" s="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -1062,10 +1095,10 @@
         <v>26</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>4</v>
@@ -1073,8 +1106,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creating the 2nd scenario of CourtOrder
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite CourtOrder AEO1971civildebt201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite CourtOrder AEO1971civildebt201819.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>TC</t>
   </si>
@@ -618,7 +618,7 @@
     <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.11328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>